<commit_message>
commit 1 bien code
</commit_message>
<xml_diff>
--- a/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
+++ b/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
@@ -770,23 +770,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="106.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="31.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
@@ -795,7 +797,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -811,8 +813,11 @@
       <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>20140707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -829,7 +834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -846,7 +851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -863,7 +868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -880,7 +885,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -897,7 +902,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -912,7 +917,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -927,7 +932,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -942,7 +947,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -959,7 +964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -976,7 +981,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -993,7 +998,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -1117,7 +1122,7 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -1164,7 +1169,7 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>22</v>
       </c>
@@ -1196,7 +1201,7 @@
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>24</v>
       </c>
@@ -1213,7 +1218,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>25</v>
       </c>
@@ -1230,7 +1235,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>26</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>27</v>
       </c>
@@ -1262,7 +1267,7 @@
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>28</v>
       </c>
@@ -1279,7 +1284,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>29</v>
       </c>
@@ -1311,7 +1316,7 @@
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>31</v>
       </c>
@@ -1328,7 +1333,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>32</v>
       </c>
@@ -1375,7 +1380,7 @@
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
commit src cho phần cart
</commit_message>
<xml_diff>
--- a/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
+++ b/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$E$40</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>STT</t>
   </si>
@@ -228,6 +231,15 @@
   </si>
   <si>
     <t>NOTE : Ưu tiên các item có độ ưu tiên 1-2-3. 1 sẽ là bắt buộc.</t>
+  </si>
+  <si>
+    <t>ON GONING</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>ON GOING</t>
   </si>
 </sst>
 </file>
@@ -243,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +265,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +311,7 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color auto="1"/>
       </top>
       <bottom style="hair">
@@ -302,7 +326,7 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color auto="1"/>
       </top>
       <bottom style="hair">
@@ -317,7 +341,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color auto="1"/>
       </top>
       <bottom style="hair">
@@ -335,7 +359,7 @@
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -350,7 +374,7 @@
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -365,7 +389,7 @@
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -377,10 +401,8 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -392,10 +414,8 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -407,10 +427,8 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -419,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -436,9 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -448,26 +463,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,634 +828,749 @@
     <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1">
-        <v>20140707</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="F3" s="9">
+        <v>20140803</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="F4" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="F5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="F6" s="3"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="F7" s="3"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="F8" s="3"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="16">
         <v>2</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="E11" s="16"/>
+      <c r="F11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="F12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="F13" s="3"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="F14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="7">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
+      <c r="F15" s="3"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="3">
         <v>4</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="F16" s="3"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="F17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="F18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="3">
         <v>4</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <v>16</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="16">
         <v>2</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="E20" s="16"/>
+      <c r="F20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <v>17</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="D21" s="16">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>18</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>19</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="3">
         <v>2</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="F23" s="3"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="3">
         <v>3</v>
       </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <v>22</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="7">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="16">
+        <v>1</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="F26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="7">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <v>24</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="D28" s="13">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="F28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>25</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-      <c r="E29" s="9" t="s">
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="F29" s="3"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>26</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="F30" s="3"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
         <v>27</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="7">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="D31" s="13">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="3">
         <v>2</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>29</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="3">
         <v>3</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="F33" s="3"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
         <v>30</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B34" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="7">
-        <v>1</v>
-      </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
         <v>31</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="13">
         <v>2</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+      <c r="F35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
         <v>32</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="B36" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="7">
-        <v>1</v>
-      </c>
-      <c r="E36" s="9" t="s">
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="F36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>33</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="3">
         <v>2</v>
       </c>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>34</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="3">
         <v>2</v>
       </c>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>35</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="3">
         <v>3</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="F39" s="3"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
         <v>36</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="12" t="s">
+      <c r="B40" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="6">
         <v>3</v>
       </c>
-      <c r="E40" s="13"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
tích hợp nâng cao
</commit_message>
<xml_diff>
--- a/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
+++ b/docs/20140701_Phase 2/Phase2_Scope_20140703.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>STT</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Còn portal admin</t>
+  </si>
+  <si>
+    <t>Tích hợp sâu ngân lươngj</t>
   </si>
 </sst>
 </file>
@@ -490,9 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -516,6 +516,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,10 +822,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,27 +838,28 @@
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="12.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F2" s="18" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -880,32 +884,35 @@
       <c r="H3" s="1">
         <v>20140819</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21" t="s">
+      <c r="I3" s="1">
+        <v>20140904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="21">
-        <v>1</v>
-      </c>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="20">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="24"/>
+      <c r="F4" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="23"/>
       <c r="H4" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -929,7 +936,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -948,7 +955,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -967,7 +974,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -986,26 +993,29 @@
       <c r="F8" s="3"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="15">
-        <v>1</v>
-      </c>
-      <c r="E9" s="15"/>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12"/>
       <c r="F9" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1022,26 +1032,29 @@
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>8</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -1062,7 +1075,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1081,7 +1094,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>11</v>
       </c>
@@ -1102,7 +1115,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>12</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
@@ -1139,28 +1152,31 @@
       <c r="F16" s="3"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>13</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="15">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15" t="s">
+      <c r="D17" s="12">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>14</v>
       </c>
@@ -1184,7 +1200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -1201,20 +1217,20 @@
       <c r="F19" s="3"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>16</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>2</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="3" t="s">
         <v>70</v>
       </c>
@@ -1222,8 +1238,11 @@
       <c r="H20" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>17</v>
       </c>
@@ -1241,8 +1260,11 @@
         <v>70</v>
       </c>
       <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -1259,7 +1281,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1278,7 +1300,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>20</v>
       </c>
@@ -1298,7 +1320,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -1315,20 +1337,20 @@
       <c r="F25" s="3"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>22</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="15">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>43</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -1336,7 +1358,7 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -1353,7 +1375,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>24</v>
       </c>
@@ -1374,7 +1396,7 @@
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>25</v>
       </c>
@@ -1396,7 +1418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -1415,7 +1437,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>27</v>
       </c>
@@ -1434,7 +1456,7 @@
       </c>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -1453,7 +1475,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -1472,7 +1494,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>30</v>
       </c>
@@ -1491,7 +1513,7 @@
       </c>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>31</v>
       </c>
@@ -1512,28 +1534,31 @@
       </c>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>32</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="17" t="s">
+      <c r="B36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="15">
-        <v>1</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="D36" s="12">
+        <v>1</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>33</v>
       </c>
@@ -1551,8 +1576,11 @@
       <c r="G37" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -1569,7 +1597,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>35</v>
       </c>
@@ -1588,7 +1616,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>36</v>
       </c>
@@ -1604,6 +1632,20 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>35</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:G40">

</xml_diff>